<commit_message>
refactors to use fixed Excel-System
</commit_message>
<xml_diff>
--- a/src/test/data/railway/Railway.xlsx
+++ b/src/test/data/railway/Railway.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="34720" yWindow="-13260" windowWidth="25600" windowHeight="16060" tabRatio="363" activeTab="1"/>
+    <workbookView xWindow="-28340" yWindow="-11560" windowWidth="25600" windowHeight="16060" tabRatio="363" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="City" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Aachen</t>
   </si>
@@ -71,12 +71,6 @@
     <t>Line-number</t>
   </si>
   <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -147,14 +141,24 @@
   </si>
   <si>
     <t>Stolberg Hbf</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>in (City)</t>
+  </si>
+  <si>
+    <t>out (City)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -199,7 +203,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -211,8 +215,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -222,18 +230,25 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -623,7 +638,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -631,165 +646,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A14" sqref="A14:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1">
+      <c r="A1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>50.776667000000003</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>6.0836110000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="7">
+        <f>A2+1</f>
+        <v>1001</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>50.8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>6.483333</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="7">
+        <f t="shared" ref="A4:A13" si="0">A3+1</f>
+        <v>1002</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>51.225555999999997</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>6.7827780000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="7">
+        <f t="shared" si="0"/>
+        <v>1003</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>50.820833</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>6.2630559999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="7">
+        <f t="shared" si="0"/>
+        <v>1004</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>50.965277999999998</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>6.1194439999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="7">
+        <f t="shared" si="0"/>
+        <v>1005</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>50.866667</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>6.1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="7">
+        <f t="shared" si="0"/>
+        <v>1006</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>50.938056000000003</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>6.956944</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="7">
+        <f t="shared" si="0"/>
+        <v>1007</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>51.336944000000003</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>6.5641670000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="7">
+        <f t="shared" si="0"/>
+        <v>1008</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>50.816667000000002</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>6.3497219999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="7">
+        <f t="shared" si="0"/>
+        <v>1009</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>51.191110999999999</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>6.4419440000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" s="7">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>51.198611</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>6.691389</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="7">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>50.766666999999998</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>6.233333</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="C14" s="1"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -809,333 +872,408 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="7">
+        <v>2000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D2">
+        <v>50.768056000000001</v>
+      </c>
+      <c r="E2">
+        <v>6.0911109999999997</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7">
+        <f>A2+1</f>
+        <v>2001</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C2">
-        <v>50.768056000000001</v>
-      </c>
-      <c r="D2">
-        <v>6.0911109999999997</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D3">
+        <v>50.78</v>
+      </c>
+      <c r="E3">
+        <v>6.0711110000000001</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="7">
+        <f t="shared" ref="A4:A19" si="0">A3+1</f>
+        <v>2002</v>
+      </c>
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C3">
-        <v>50.78</v>
-      </c>
-      <c r="D3">
-        <v>6.0711110000000001</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D4">
+        <v>50.769975000000002</v>
+      </c>
+      <c r="E4">
+        <v>6.0737249999999996</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="D5">
+        <v>50.770339999999997</v>
+      </c>
+      <c r="E5">
+        <v>6.1162999999999998</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+      <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>50.785556</v>
+      </c>
+      <c r="E6">
+        <v>6.1545829999999997</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C4">
-        <v>50.769975000000002</v>
-      </c>
-      <c r="D4">
-        <v>6.0737249999999996</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5">
-        <v>50.770339999999997</v>
-      </c>
-      <c r="D5">
-        <v>6.1162999999999998</v>
-      </c>
-      <c r="E5" s="4" t="s">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="7">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D7">
+        <v>50.810833000000002</v>
+      </c>
+      <c r="E7">
+        <v>6.4824999999999999</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6">
-        <v>50.785556</v>
-      </c>
-      <c r="D6">
-        <v>6.1545829999999997</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="7">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C7">
-        <v>50.810833000000002</v>
-      </c>
-      <c r="D7">
-        <v>6.4824999999999999</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D8">
+        <v>51.220278</v>
+      </c>
+      <c r="E8">
+        <v>6.7927780000000002</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="7">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D9">
+        <v>50.813333</v>
+      </c>
+      <c r="E9">
+        <v>6.2522219999999997</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="7">
+        <f t="shared" si="0"/>
+        <v>2008</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="C8">
-        <v>51.220278</v>
-      </c>
-      <c r="D8">
-        <v>6.7927780000000002</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D10">
+        <v>50.961111000000002</v>
+      </c>
+      <c r="E10">
+        <v>6.1241669999999999</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="7">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="C9">
-        <v>50.813333</v>
-      </c>
-      <c r="D9">
-        <v>6.2522219999999997</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D11">
+        <v>50.870832999999998</v>
+      </c>
+      <c r="E11">
+        <v>6.0946389999999999</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="7">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="C10">
-        <v>50.961111000000002</v>
-      </c>
-      <c r="D10">
-        <v>6.1241669999999999</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="7">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="C11">
-        <v>50.870832999999998</v>
-      </c>
-      <c r="D11">
-        <v>6.0946389999999999</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D13">
+        <v>50.942500000000003</v>
+      </c>
+      <c r="E13">
+        <v>6.958056</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D14">
+        <v>50.946389000000003</v>
+      </c>
+      <c r="E14">
+        <v>6.9183329999999996</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="7">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="C13">
-        <v>50.942500000000003</v>
-      </c>
-      <c r="D13">
-        <v>6.958056</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D15">
+        <v>51.325833000000003</v>
+      </c>
+      <c r="E15">
+        <v>6.5694439999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="7">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="C14">
-        <v>50.946389000000003</v>
-      </c>
-      <c r="D14">
-        <v>6.9183329999999996</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D16">
+        <v>50.817447000000001</v>
+      </c>
+      <c r="E16">
+        <v>6.3551650000000004</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="7">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="C15">
-        <v>51.325833000000003</v>
-      </c>
-      <c r="D15">
-        <v>6.5694439999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D17">
+        <v>51.196389000000003</v>
+      </c>
+      <c r="E17">
+        <v>6.4461110000000001</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="7">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="C16">
-        <v>50.817447000000001</v>
-      </c>
-      <c r="D16">
-        <v>6.3551650000000004</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D18">
+        <v>51.204166999999998</v>
+      </c>
+      <c r="E18">
+        <v>6.6838889999999997</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="7">
+        <f t="shared" si="0"/>
+        <v>2017</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="C17">
-        <v>51.196389000000003</v>
-      </c>
-      <c r="D17">
-        <v>6.4461110000000001</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18">
-        <v>51.204166999999998</v>
-      </c>
-      <c r="D18">
-        <v>6.6838889999999997</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19">
+      <c r="D19">
         <v>50.794722</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>6.2194440000000002</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>26</v>
+      <c r="F19" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1156,72 +1294,91 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="8" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
+      <c r="C1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7">
+        <v>3000</v>
+      </c>
+      <c r="B2" s="7">
         <v>2550</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+      <c r="C2" s="7">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7">
+        <f>A2+1</f>
+        <v>3001</v>
+      </c>
+      <c r="B3" s="7">
         <v>2550</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="C3" s="7">
+        <v>1009</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7">
+        <f t="shared" ref="A4:A5" si="0">A3+1</f>
+        <v>3002</v>
+      </c>
+      <c r="B4" s="7">
         <v>2600</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="C4" s="7">
+        <v>1006</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="7">
+        <f t="shared" si="0"/>
+        <v>3003</v>
+      </c>
+      <c r="B5" s="7">
         <v>2622</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
+      <c r="C5" s="7">
+        <v>1006</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>